<commit_message>
Cuong fix table thiet_bi
</commit_message>
<xml_diff>
--- a/app_qly_thuquan/FileExcels/Nhập excel thiết bị.xlsx
+++ b/app_qly_thuquan/FileExcels/Nhập excel thiết bị.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1ca77da928176da/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{D1824D09-2960-4282-82EC-22D09972C6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6C3FE5A-1F2E-41D8-8C25-E49A6393B7A5}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{D1824D09-2960-4282-82EC-22D09972C6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86F99960-6572-451F-A18D-915DB28CAFCD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA9F8CA9-A886-4AFB-BECE-9AC630849014}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Tên</t>
   </si>
@@ -44,34 +44,67 @@
     <t>Nhập danh sách thiết bị</t>
   </si>
   <si>
-    <t xml:space="preserve">Máy 11  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Máy 12  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Máy 13  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Máy 14  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Máy 15  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Máy 16  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Máy 17  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Máy 18  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Máy 19  </t>
-  </si>
-  <si>
-    <t>Máy 20</t>
+    <t>Mã</t>
+  </si>
+  <si>
+    <t>MT_011</t>
+  </si>
+  <si>
+    <t>Máy tính 11</t>
+  </si>
+  <si>
+    <t>MT_012</t>
+  </si>
+  <si>
+    <t>Máy tính 12</t>
+  </si>
+  <si>
+    <t>MT_013</t>
+  </si>
+  <si>
+    <t>Máy tính 13</t>
+  </si>
+  <si>
+    <t>MT_014</t>
+  </si>
+  <si>
+    <t>Máy tính 14</t>
+  </si>
+  <si>
+    <t>MT_015</t>
+  </si>
+  <si>
+    <t>Máy tính 15</t>
+  </si>
+  <si>
+    <t>MT_016</t>
+  </si>
+  <si>
+    <t>Máy tính 16</t>
+  </si>
+  <si>
+    <t>MT_017</t>
+  </si>
+  <si>
+    <t>Máy tính 17</t>
+  </si>
+  <si>
+    <t>MT_018</t>
+  </si>
+  <si>
+    <t>Máy tính 18</t>
+  </si>
+  <si>
+    <t>MT_019</t>
+  </si>
+  <si>
+    <t>Máy tính 20</t>
+  </si>
+  <si>
+    <t>Máy tính 19</t>
+  </si>
+  <si>
+    <t>MT_020</t>
   </si>
 </sst>
 </file>
@@ -115,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -123,7 +156,12 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -461,79 +499,116 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>10</v>
+      <c r="A11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
+      <c r="A12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>